<commit_message>
Inhaltsverzeichnis im Bereich Geschichte angepasst
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Datum</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Der Endtermin wurde extra früher verlegt, damit genug Zeit für Verschiebungen und Überarbeitungen vorhanden ist</t>
+  </si>
+  <si>
+    <t>Schlusspräsentation</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -65,7 +71,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -112,14 +118,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -414,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -427,24 +436,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33.75" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>40791</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -496,10 +505,10 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>40847</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -530,10 +539,10 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>40882</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -545,13 +554,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Geschichte der klassischen Kryptographie und Abgabetermin im Zeitplan angepasst
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="15315" windowHeight="7740"/>
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Datum</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Definitive Abgabe der Maturaarbeit</t>
   </si>
 </sst>
 </file>
@@ -118,17 +121,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -423,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -436,10 +440,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33.75" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
@@ -555,20 +559,28 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6">
+        <v>40896</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
@@ -577,7 +589,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>